<commit_message>
just test excel to bin success
</commit_message>
<xml_diff>
--- a/Resource/config/excel/hero_config_race.xlsx
+++ b/Resource/config/excel/hero_config_race.xlsx
@@ -12,90 +12,53 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>顺序</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>职业名字</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_name</t>
   </si>
   <si>
     <t>id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>display_name</t>
-  </si>
-  <si>
-    <t>type_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Human</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mask</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lizard</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Snow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giant</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>人类</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>蜥蜴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>雪人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>巨人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐士</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0type_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -125,11 +88,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -462,148 +422,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B9" s="1">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B10" s="1">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B11" s="1">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B12" s="1">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B13" s="1">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
debug excel to bin success , but have a bug still
</commit_message>
<xml_diff>
--- a/Resource/config/excel/hero_config_race.xlsx
+++ b/Resource/config/excel/hero_config_race.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -27,24 +27,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>职业名字</t>
+  </si>
+  <si>
+    <t>www</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rrr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>display_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>顺序</t>
-  </si>
-  <si>
-    <t>职业名字</t>
-  </si>
-  <si>
-    <t>display_name</t>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0type_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,7 +431,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -436,9 +442,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -446,8 +458,14 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -455,10 +473,10 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -489,10 +507,10 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -512,10 +530,10 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>24</v>
+        <v>424</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>